<commit_message>
allow superusers to see link and hide questionnum if not used by default
</commit_message>
<xml_diff>
--- a/assets/TestProjectGenerator.xlsx
+++ b/assets/TestProjectGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy123/Projects/redcap-local/modules-local/shazam_v0.0.0/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100008_{BBAC72F2-1C27-8447-AD73-970CA9607E22}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100008_{F5459E1C-9054-EB4A-AA46-59710B6C57BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="4060" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{AF6DBCE9-EA33-004C-954B-8E6178EA0CD7}"/>
+    <workbookView xWindow="5980" yWindow="4060" windowWidth="27240" windowHeight="16440" xr2:uid="{AF6DBCE9-EA33-004C-954B-8E6178EA0CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="SHAZAM HTML" sheetId="1" r:id="rId1"/>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDAD074-C32A-4B48-8280-93EA274611E9}">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2092,11 +2092,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2AAF2F-8E4C-914D-A386-BAE1DACBEB31}">
   <dimension ref="A1:R137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44:F47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>